<commit_message>
Update data, maps, pages
</commit_message>
<xml_diff>
--- a/data/source/reference/chicago_category_notes_analysis.xlsx
+++ b/data/source/reference/chicago_category_notes_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Jarvis/R/safetytracker_chicago/data/source/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED96298-1EB4-9B46-A89D-F32CFF48F577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267A51FB-B22C-5249-B468-96ACE31F4620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41660" yWindow="4300" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{2D38F7AF-362E-284B-8B20-3A7554E5C55D}"/>
+    <workbookView xWindow="27680" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{2D38F7AF-362E-284B-8B20-3A7554E5C55D}"/>
   </bookViews>
   <sheets>
     <sheet name="rape cats" sheetId="1" r:id="rId1"/>
@@ -2181,7 +2181,7 @@
     <t>Vacant Lot</t>
   </si>
   <si>
-    <t>case_when(chicago_crime$location_description == '</t>
+    <t>(chicago_crime$location_description == '</t>
   </si>
 </sst>
 </file>
@@ -8588,7 +8588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFE5826-9C8D-BD43-AF0B-A1E294847A4B}">
   <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C166" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F174"/>
     </sheetView>
   </sheetViews>
@@ -8630,7 +8630,7 @@
       </c>
       <c r="F3" t="str">
         <f>C3&amp;D3&amp;"' ~ '"&amp;E3&amp;"',"</f>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT BUILDING NON-TERMINAL - NON-SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT BUILDING NON-TERMINAL - NON-SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -8649,7 +8649,7 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F67" si="0">C4&amp;D4&amp;"' ~ '"&amp;E4&amp;"',"</f>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT BUILDING NON-TERMINAL - SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT BUILDING NON-TERMINAL - SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -8668,7 +8668,7 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT EXTERIOR - NON-SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT EXTERIOR - NON-SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT EXTERIOR - SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT EXTERIOR - SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -8706,7 +8706,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT PARKING LOT' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT PARKING LOT' ~ 'Airport',</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -8725,7 +8725,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT TERMINAL LOWER LEVEL - NON-SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT TERMINAL LOWER LEVEL - NON-SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -8744,7 +8744,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT TERMINAL LOWER LEVEL - SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT TERMINAL LOWER LEVEL - SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT TERMINAL MEZZANINE - NON-SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT TERMINAL MEZZANINE - NON-SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8782,7 +8782,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT TERMINAL UPPER LEVEL - NON-SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT TERMINAL UPPER LEVEL - NON-SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -8801,7 +8801,7 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT TERMINAL UPPER LEVEL - SECURE AREA' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT TERMINAL UPPER LEVEL - SECURE AREA' ~ 'Airport',</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -8820,7 +8820,7 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT TRANSPORTATION SYSTEM (ATS)' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT TRANSPORTATION SYSTEM (ATS)' ~ 'Airport',</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -8839,7 +8839,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT VENDING ESTABLISHMENT' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT VENDING ESTABLISHMENT' ~ 'Airport',</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -8858,7 +8858,7 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AIRPORT/AIRCRAFT' ~ 'Airport',</v>
+        <v>(chicago_crime$location_description == 'AIRPORT/AIRCRAFT' ~ 'Airport',</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -8877,7 +8877,7 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'ANIMAL HOSPITAL' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'ANIMAL HOSPITAL' ~ 'Business',</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -8896,7 +8896,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'APARTMENT' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'APARTMENT' ~ 'Residence',</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -8915,7 +8915,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'APPLIANCE STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'APPLIANCE STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -8934,7 +8934,7 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'ATHLETIC CLUB' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'ATHLETIC CLUB' ~ 'Business',</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -8953,7 +8953,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'ATM (AUTOMATIC TELLER MACHINE)' ~ 'Bank',</v>
+        <v>(chicago_crime$location_description == 'ATM (AUTOMATIC TELLER MACHINE)' ~ 'Bank',</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -8972,7 +8972,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AUTO' ~ 'Automobile',</v>
+        <v>(chicago_crime$location_description == 'AUTO' ~ 'Automobile',</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -8991,7 +8991,7 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'AUTO / BOAT / RV DEALERSHIP' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'AUTO / BOAT / RV DEALERSHIP' ~ 'Business',</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -9010,7 +9010,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BANK' ~ 'Bank',</v>
+        <v>(chicago_crime$location_description == 'BANK' ~ 'Bank',</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -9029,7 +9029,7 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BANQUET HALL' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'BANQUET HALL' ~ 'Business',</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -9048,7 +9048,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BAR OR TAVERN' ~ 'Bar, Tavern or Club',</v>
+        <v>(chicago_crime$location_description == 'BAR OR TAVERN' ~ 'Bar, Tavern or Club',</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -9067,7 +9067,7 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BARBER SHOP/BEAUTY SALON' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'BARBER SHOP/BEAUTY SALON' ~ 'Business',</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -9086,7 +9086,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BARBERSHOP' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'BARBERSHOP' ~ 'Business',</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -9105,7 +9105,7 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BASEMENT' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'BASEMENT' ~ 'Residence',</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -9124,7 +9124,7 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BOAT / WATERCRAFT' ~ 'Watercraft',</v>
+        <v>(chicago_crime$location_description == 'BOAT / WATERCRAFT' ~ 'Watercraft',</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -9143,7 +9143,7 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BOAT/WATERCRAFT' ~ 'Watercraft',</v>
+        <v>(chicago_crime$location_description == 'BOAT/WATERCRAFT' ~ 'Watercraft',</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -9162,7 +9162,7 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'BOWLING ALLEY' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'BOWLING ALLEY' ~ 'Business',</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -9181,7 +9181,7 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CAR WASH' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'CAR WASH' ~ 'Business',</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -9200,7 +9200,7 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA APARTMENT' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA APARTMENT' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -9219,7 +9219,7 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA ELEVATOR' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA ELEVATOR' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -9238,7 +9238,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA GROUNDS' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA GROUNDS' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -9257,7 +9257,7 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA HALLWAY' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA HALLWAY' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -9276,7 +9276,7 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA HALLWAY / STAIRWELL / ELEVATOR' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA HALLWAY / STAIRWELL / ELEVATOR' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -9295,7 +9295,7 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA HALLWAY/STAIRWELL/ELEVATOR' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA HALLWAY/STAIRWELL/ELEVATOR' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA LOBBY' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA LOBBY' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -9333,7 +9333,7 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA PARKING LOT' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA PARKING LOT' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -9352,7 +9352,7 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA PARKING LOT / GROUNDS' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA PARKING LOT / GROUNDS' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA PARKING LOT/GROUNDS' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA PARKING LOT/GROUNDS' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -9390,7 +9390,7 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHA PLAY LOT' ~ 'Housing Authority',</v>
+        <v>(chicago_crime$location_description == 'CHA PLAY LOT' ~ 'Housing Authority',</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -9409,7 +9409,7 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHURCH / SYNAGOGUE / PLACE OF WORSHIP' ~ 'Place of Worship',</v>
+        <v>(chicago_crime$location_description == 'CHURCH / SYNAGOGUE / PLACE OF WORSHIP' ~ 'Place of Worship',</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -9428,7 +9428,7 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CHURCH/SYNAGOGUE/PLACE OF WORSHIP' ~ 'Place of Worship',</v>
+        <v>(chicago_crime$location_description == 'CHURCH/SYNAGOGUE/PLACE OF WORSHIP' ~ 'Place of Worship',</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -9447,7 +9447,7 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CLEANING STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'CLEANING STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -9466,7 +9466,7 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CLUB' ~ 'Bar, Tavern or Club',</v>
+        <v>(chicago_crime$location_description == 'CLUB' ~ 'Bar, Tavern or Club',</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -9485,7 +9485,7 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'COIN OPERATED MACHINE' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'COIN OPERATED MACHINE' ~ 'Other',</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -9504,7 +9504,7 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'COLLEGE / UNIVERSITY - GROUNDS' ~ 'College or University',</v>
+        <v>(chicago_crime$location_description == 'COLLEGE / UNIVERSITY - GROUNDS' ~ 'College or University',</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -9523,7 +9523,7 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'COLLEGE / UNIVERSITY - RESIDENCE HALL' ~ 'College or University',</v>
+        <v>(chicago_crime$location_description == 'COLLEGE / UNIVERSITY - RESIDENCE HALL' ~ 'College or University',</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -9542,7 +9542,7 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'COLLEGE/UNIVERSITY GROUNDS' ~ 'College or University',</v>
+        <v>(chicago_crime$location_description == 'COLLEGE/UNIVERSITY GROUNDS' ~ 'College or University',</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -9561,7 +9561,7 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'COLLEGE/UNIVERSITY RESIDENCE HALL' ~ 'College or University',</v>
+        <v>(chicago_crime$location_description == 'COLLEGE/UNIVERSITY RESIDENCE HALL' ~ 'College or University',</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -9580,7 +9580,7 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'COMMERCIAL / BUSINESS OFFICE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'COMMERCIAL / BUSINESS OFFICE' ~ 'Business',</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -9599,7 +9599,7 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CONVENIENCE STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'CONVENIENCE STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -9618,7 +9618,7 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CREDIT UNION' ~ 'Bank',</v>
+        <v>(chicago_crime$location_description == 'CREDIT UNION' ~ 'Bank',</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -9637,7 +9637,7 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA "L" PLATFORM' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA "L" PLATFORM' ~ 'Transit',</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -9656,7 +9656,7 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA "L" TRAIN' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA "L" TRAIN' ~ 'Transit',</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -9675,7 +9675,7 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA BUS' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA BUS' ~ 'Transit',</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -9694,7 +9694,7 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA BUS STOP' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA BUS STOP' ~ 'Transit',</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -9713,7 +9713,7 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA GARAGE / OTHER PROPERTY' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA GARAGE / OTHER PROPERTY' ~ 'Transit',</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -9732,7 +9732,7 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA PARKING LOT / GARAGE / OTHER PROPERTY' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA PARKING LOT / GARAGE / OTHER PROPERTY' ~ 'Transit',</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -9751,7 +9751,7 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA PLATFORM' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA PLATFORM' ~ 'Transit',</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -9770,7 +9770,7 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA PROPERTY' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA PROPERTY' ~ 'Transit',</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -9789,7 +9789,7 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA STATION' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA STATION' ~ 'Transit',</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -9808,7 +9808,7 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA SUBWAY STATION' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA SUBWAY STATION' ~ 'Transit',</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -9827,7 +9827,7 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA TRACKS - RIGHT OF WAY' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA TRACKS - RIGHT OF WAY' ~ 'Transit',</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -9846,7 +9846,7 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v>case_when(chicago_crime$location_description == 'CTA TRAIN' ~ 'Transit',</v>
+        <v>(chicago_crime$location_description == 'CTA TRAIN' ~ 'Transit',</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" ref="F68:F131" si="1">C68&amp;D68&amp;"' ~ '"&amp;E68&amp;"',"</f>
-        <v>case_when(chicago_crime$location_description == 'CURRENCY EXCHANGE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'CURRENCY EXCHANGE' ~ 'Business',</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -9884,7 +9884,7 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'DAY CARE CENTER' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'DAY CARE CENTER' ~ 'Business',</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -9903,7 +9903,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'DEPARTMENT STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'DEPARTMENT STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -9922,7 +9922,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'DRIVEWAY' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'DRIVEWAY' ~ 'Other',</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -9941,7 +9941,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'DRIVEWAY - RESIDENTIAL' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'DRIVEWAY - RESIDENTIAL' ~ 'Residence',</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -9960,7 +9960,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'DRUG STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'DRUG STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -9979,7 +9979,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'ELEVATOR' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'ELEVATOR' ~ 'Other',</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -9998,7 +9998,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'FACTORY / MANUFACTURING BUILDING' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'FACTORY / MANUFACTURING BUILDING' ~ 'Business',</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -10017,7 +10017,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'FACTORY/MANUFACTURING BUILDING' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'FACTORY/MANUFACTURING BUILDING' ~ 'Business',</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -10036,7 +10036,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'FEDERAL BUILDING' ~ 'Government Building or Property',</v>
+        <v>(chicago_crime$location_description == 'FEDERAL BUILDING' ~ 'Government Building or Property',</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -10055,7 +10055,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'FIRE STATION' ~ 'Government Building or Property',</v>
+        <v>(chicago_crime$location_description == 'FIRE STATION' ~ 'Government Building or Property',</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -10074,7 +10074,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'FOREST PRESERVE' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'FOREST PRESERVE' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -10093,7 +10093,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GANGWAY' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'GANGWAY' ~ 'Other',</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -10112,7 +10112,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GARAGE' ~ 'Parking Lot/Garage',</v>
+        <v>(chicago_crime$location_description == 'GARAGE' ~ 'Parking Lot/Garage',</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -10131,7 +10131,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GAS STATION' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'GAS STATION' ~ 'Business',</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -10150,7 +10150,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GAS STATION DRIVE/PROP.' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'GAS STATION DRIVE/PROP.' ~ 'Business',</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -10169,7 +10169,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GOVERNMENT BUILDING / PROPERTY' ~ 'Government Building or Property',</v>
+        <v>(chicago_crime$location_description == 'GOVERNMENT BUILDING / PROPERTY' ~ 'Government Building or Property',</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -10188,7 +10188,7 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GOVERNMENT BUILDING/PROPERTY' ~ 'Government Building or Property',</v>
+        <v>(chicago_crime$location_description == 'GOVERNMENT BUILDING/PROPERTY' ~ 'Government Building or Property',</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -10207,7 +10207,7 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'GROCERY FOOD STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'GROCERY FOOD STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -10226,7 +10226,7 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HALLWAY' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'HALLWAY' ~ 'Other',</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -10245,7 +10245,7 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HIGHWAY / EXPRESSWAY' ~ 'Street or Highway',</v>
+        <v>(chicago_crime$location_description == 'HIGHWAY / EXPRESSWAY' ~ 'Street or Highway',</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -10264,7 +10264,7 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HIGHWAY/EXPRESSWAY' ~ 'Street or Highway',</v>
+        <v>(chicago_crime$location_description == 'HIGHWAY/EXPRESSWAY' ~ 'Street or Highway',</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -10283,7 +10283,7 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HORSE STABLE' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'HORSE STABLE' ~ 'Other',</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -10302,7 +10302,7 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOSPITAL' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'HOSPITAL' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -10321,7 +10321,7 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOSPITAL BUILDING / GROUNDS' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'HOSPITAL BUILDING / GROUNDS' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -10340,7 +10340,7 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOSPITAL BUILDING/GROUNDS' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'HOSPITAL BUILDING/GROUNDS' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -10359,7 +10359,7 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOTEL' ~ 'Hotel or Motel',</v>
+        <v>(chicago_crime$location_description == 'HOTEL' ~ 'Hotel or Motel',</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -10378,7 +10378,7 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOTEL / MOTEL' ~ 'Hotel or Motel',</v>
+        <v>(chicago_crime$location_description == 'HOTEL / MOTEL' ~ 'Hotel or Motel',</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -10397,7 +10397,7 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOTEL/MOTEL' ~ 'Hotel or Motel',</v>
+        <v>(chicago_crime$location_description == 'HOTEL/MOTEL' ~ 'Hotel or Motel',</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -10416,7 +10416,7 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'HOUSE' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'HOUSE' ~ 'Residence',</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -10435,7 +10435,7 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'JAIL / LOCK-UP FACILITY' ~ 'Jail or Prison',</v>
+        <v>(chicago_crime$location_description == 'JAIL / LOCK-UP FACILITY' ~ 'Jail or Prison',</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -10454,7 +10454,7 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'KENNEL' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'KENNEL' ~ 'Other',</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -10473,7 +10473,7 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'LAKE' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'LAKE' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -10492,7 +10492,7 @@
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'LAKEFRONT / WATERFRONT / RIVERBANK' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'LAKEFRONT / WATERFRONT / RIVERBANK' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'LAKEFRONT/WATERFRONT/RIVERBANK' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'LAKEFRONT/WATERFRONT/RIVERBANK' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -10530,7 +10530,7 @@
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'LIBRARY' ~ 'Government Building or Property',</v>
+        <v>(chicago_crime$location_description == 'LIBRARY' ~ 'Government Building or Property',</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -10549,7 +10549,7 @@
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'LIQUOR STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'LIQUOR STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -10568,7 +10568,7 @@
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'MEDICAL / DENTAL OFFICE' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'MEDICAL / DENTAL OFFICE' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -10587,7 +10587,7 @@
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'MEDICAL/DENTAL OFFICE' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'MEDICAL/DENTAL OFFICE' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -10606,7 +10606,7 @@
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'MOTEL' ~ 'Hotel or Motel',</v>
+        <v>(chicago_crime$location_description == 'MOTEL' ~ 'Hotel or Motel',</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -10625,7 +10625,7 @@
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'MOVIE HOUSE / THEATER' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'MOVIE HOUSE / THEATER' ~ 'Business',</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -10644,7 +10644,7 @@
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'MOVIE HOUSE/THEATER' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'MOVIE HOUSE/THEATER' ~ 'Business',</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -10663,7 +10663,7 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'NEWSSTAND' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'NEWSSTAND' ~ 'Business',</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -10682,7 +10682,7 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'NURSING / RETIREMENT HOME' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'NURSING / RETIREMENT HOME' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -10701,7 +10701,7 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'NURSING HOME' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'NURSING HOME' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -10720,7 +10720,7 @@
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'NURSING HOME/RETIREMENT HOME' ~ 'Medical Facility',</v>
+        <v>(chicago_crime$location_description == 'NURSING HOME/RETIREMENT HOME' ~ 'Medical Facility',</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -10739,7 +10739,7 @@
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'OFFICE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'OFFICE' ~ 'Business',</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -10758,7 +10758,7 @@
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'OTHER (SPECIFY)' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'OTHER (SPECIFY)' ~ 'Other',</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -10777,7 +10777,7 @@
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'OTHER COMMERCIAL TRANSPORTATION' ~ 'Other Transportation Facility',</v>
+        <v>(chicago_crime$location_description == 'OTHER COMMERCIAL TRANSPORTATION' ~ 'Other Transportation Facility',</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -10796,7 +10796,7 @@
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'OTHER RAILROAD PROP / TRAIN DEPOT' ~ 'Other Transportation Facility',</v>
+        <v>(chicago_crime$location_description == 'OTHER RAILROAD PROP / TRAIN DEPOT' ~ 'Other Transportation Facility',</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -10815,7 +10815,7 @@
       </c>
       <c r="F118" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'OTHER RAILROAD PROPERTY / TRAIN DEPOT' ~ 'Other Transportation Facility',</v>
+        <v>(chicago_crime$location_description == 'OTHER RAILROAD PROPERTY / TRAIN DEPOT' ~ 'Other Transportation Facility',</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -10834,7 +10834,7 @@
       </c>
       <c r="F119" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'PARK PROPERTY' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'PARK PROPERTY' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -10853,7 +10853,7 @@
       </c>
       <c r="F120" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'PARKING LOT' ~ 'Parking Lot/Garage',</v>
+        <v>(chicago_crime$location_description == 'PARKING LOT' ~ 'Parking Lot/Garage',</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -10872,7 +10872,7 @@
       </c>
       <c r="F121" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'PARKING LOT / GARAGE (NON RESIDENTIAL)' ~ 'Parking Lot/Garage',</v>
+        <v>(chicago_crime$location_description == 'PARKING LOT / GARAGE (NON RESIDENTIAL)' ~ 'Parking Lot/Garage',</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -10891,7 +10891,7 @@
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'PARKING LOT/GARAGE(NON.RESID.)' ~ 'Parking Lot/Garage',</v>
+        <v>(chicago_crime$location_description == 'PARKING LOT/GARAGE(NON.RESID.)' ~ 'Parking Lot/Garage',</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -10910,7 +10910,7 @@
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'PAWN SHOP' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'PAWN SHOP' ~ 'Business',</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -10929,7 +10929,7 @@
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'POLICE FACILITY / VEHICLE PARKING LOT' ~ 'Police Facility',</v>
+        <v>(chicago_crime$location_description == 'POLICE FACILITY / VEHICLE PARKING LOT' ~ 'Police Facility',</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -10948,7 +10948,7 @@
       </c>
       <c r="F125" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'POLICE FACILITY/VEH PARKING LOT' ~ 'Police Facility',</v>
+        <v>(chicago_crime$location_description == 'POLICE FACILITY/VEH PARKING LOT' ~ 'Police Facility',</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -10967,7 +10967,7 @@
       </c>
       <c r="F126" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'POOL ROOM' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'POOL ROOM' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="F127" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'PORCH' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'PORCH' ~ 'Residence',</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -11005,7 +11005,7 @@
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'RAILROAD PROPERTY' ~ 'Other Transportation Facility',</v>
+        <v>(chicago_crime$location_description == 'RAILROAD PROPERTY' ~ 'Other Transportation Facility',</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -11024,7 +11024,7 @@
       </c>
       <c r="F129" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'RESIDENCE' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENCE' ~ 'Residence',</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -11043,7 +11043,7 @@
       </c>
       <c r="F130" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'RESIDENCE - GARAGE' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENCE - GARAGE' ~ 'Residence',</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -11062,7 +11062,7 @@
       </c>
       <c r="F131" t="str">
         <f t="shared" si="1"/>
-        <v>case_when(chicago_crime$location_description == 'RESIDENCE - PORCH / HALLWAY' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENCE - PORCH / HALLWAY' ~ 'Residence',</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -11081,7 +11081,7 @@
       </c>
       <c r="F132" t="str">
         <f t="shared" ref="F132:F174" si="2">C132&amp;D132&amp;"' ~ '"&amp;E132&amp;"',"</f>
-        <v>case_when(chicago_crime$location_description == 'RESIDENCE - YARD (FRONT / BACK)' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENCE - YARD (FRONT / BACK)' ~ 'Residence',</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -11100,7 +11100,7 @@
       </c>
       <c r="F133" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'RESIDENCE PORCH/HALLWAY' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENCE PORCH/HALLWAY' ~ 'Residence',</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -11119,7 +11119,7 @@
       </c>
       <c r="F134" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'RESIDENCE-GARAGE' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENCE-GARAGE' ~ 'Residence',</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -11138,7 +11138,7 @@
       </c>
       <c r="F135" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'RESIDENTIAL YARD (FRONT/BACK)' ~ 'Residence',</v>
+        <v>(chicago_crime$location_description == 'RESIDENTIAL YARD (FRONT/BACK)' ~ 'Residence',</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -11157,7 +11157,7 @@
       </c>
       <c r="F136" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'RESTAURANT' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'RESTAURANT' ~ 'Business',</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
@@ -11176,7 +11176,7 @@
       </c>
       <c r="F137" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'RETAIL STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'RETAIL STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -11195,7 +11195,7 @@
       </c>
       <c r="F138" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'RIVER BANK' ~ 'Recreation Area',</v>
+        <v>(chicago_crime$location_description == 'RIVER BANK' ~ 'Recreation Area',</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -11214,7 +11214,7 @@
       </c>
       <c r="F139" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SAVINGS AND LOAN' ~ 'Bank',</v>
+        <v>(chicago_crime$location_description == 'SAVINGS AND LOAN' ~ 'Bank',</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -11233,7 +11233,7 @@
       </c>
       <c r="F140" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL - PRIVATE BUILDING' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL - PRIVATE BUILDING' ~ 'School',</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -11252,7 +11252,7 @@
       </c>
       <c r="F141" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL - PRIVATE GROUNDS' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL - PRIVATE GROUNDS' ~ 'School',</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -11271,7 +11271,7 @@
       </c>
       <c r="F142" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL - PUBLIC BUILDING' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL - PUBLIC BUILDING' ~ 'School',</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -11290,7 +11290,7 @@
       </c>
       <c r="F143" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL - PUBLIC GROUNDS' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL - PUBLIC GROUNDS' ~ 'School',</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -11309,7 +11309,7 @@
       </c>
       <c r="F144" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL YARD' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL YARD' ~ 'School',</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -11328,7 +11328,7 @@
       </c>
       <c r="F145" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL, PRIVATE, BUILDING' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL, PRIVATE, BUILDING' ~ 'School',</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -11347,7 +11347,7 @@
       </c>
       <c r="F146" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL, PRIVATE, GROUNDS' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL, PRIVATE, GROUNDS' ~ 'School',</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -11366,7 +11366,7 @@
       </c>
       <c r="F147" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL, PUBLIC, BUILDING' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL, PUBLIC, BUILDING' ~ 'School',</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -11385,7 +11385,7 @@
       </c>
       <c r="F148" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SCHOOL, PUBLIC, GROUNDS' ~ 'School',</v>
+        <v>(chicago_crime$location_description == 'SCHOOL, PUBLIC, GROUNDS' ~ 'School',</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -11404,7 +11404,7 @@
       </c>
       <c r="F149" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SMALL RETAIL STORE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'SMALL RETAIL STORE' ~ 'Business',</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -11423,7 +11423,7 @@
       </c>
       <c r="F150" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SPORTS ARENA / STADIUM' ~ 'Sports Facility',</v>
+        <v>(chicago_crime$location_description == 'SPORTS ARENA / STADIUM' ~ 'Sports Facility',</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
@@ -11442,7 +11442,7 @@
       </c>
       <c r="F151" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'SPORTS ARENA/STADIUM' ~ 'Sports Facility',</v>
+        <v>(chicago_crime$location_description == 'SPORTS ARENA/STADIUM' ~ 'Sports Facility',</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -11461,7 +11461,7 @@
       </c>
       <c r="F152" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'STAIRWELL' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'STAIRWELL' ~ 'Other',</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -11480,7 +11480,7 @@
       </c>
       <c r="F153" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'STREET' ~ 'Street or Highway',</v>
+        <v>(chicago_crime$location_description == 'STREET' ~ 'Street or Highway',</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -11499,7 +11499,7 @@
       </c>
       <c r="F154" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'TAVERN' ~ 'Bar, Tavern or Club',</v>
+        <v>(chicago_crime$location_description == 'TAVERN' ~ 'Bar, Tavern or Club',</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -11518,7 +11518,7 @@
       </c>
       <c r="F155" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'TAVERN / LIQUOR STORE' ~ 'Bar, Tavern or Club',</v>
+        <v>(chicago_crime$location_description == 'TAVERN / LIQUOR STORE' ~ 'Bar, Tavern or Club',</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -11537,7 +11537,7 @@
       </c>
       <c r="F156" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'TAVERN/LIQUOR STORE' ~ 'Bar, Tavern or Club',</v>
+        <v>(chicago_crime$location_description == 'TAVERN/LIQUOR STORE' ~ 'Bar, Tavern or Club',</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -11556,7 +11556,7 @@
       </c>
       <c r="F157" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'TAXICAB' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'TAXICAB' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -11575,7 +11575,7 @@
       </c>
       <c r="F158" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'TRAILER' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'TRAILER' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -11594,7 +11594,7 @@
       </c>
       <c r="F159" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'TRUCK' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'TRUCK' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="F160" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VACANT LOT / LAND' ~ 'Vacant Lot',</v>
+        <v>(chicago_crime$location_description == 'VACANT LOT / LAND' ~ 'Vacant Lot',</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
@@ -11632,7 +11632,7 @@
       </c>
       <c r="F161" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VACANT LOT/LAND' ~ 'Vacant Lot',</v>
+        <v>(chicago_crime$location_description == 'VACANT LOT/LAND' ~ 'Vacant Lot',</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -11651,7 +11651,7 @@
       </c>
       <c r="F162" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE - COMMERCIAL' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE - COMMERCIAL' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -11670,7 +11670,7 @@
       </c>
       <c r="F163" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE - COMMERCIAL: ENTERTAINMENT / PARTY BUS' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE - COMMERCIAL: ENTERTAINMENT / PARTY BUS' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
@@ -11689,7 +11689,7 @@
       </c>
       <c r="F164" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE - COMMERCIAL: TROLLEY BUS' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE - COMMERCIAL: TROLLEY BUS' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -11708,7 +11708,7 @@
       </c>
       <c r="F165" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE - DELIVERY TRUCK' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE - DELIVERY TRUCK' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
@@ -11727,7 +11727,7 @@
       </c>
       <c r="F166" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE - OTHER RIDE SHARE SERVICE (E.G., UBER, LYFT)' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE - OTHER RIDE SHARE SERVICE (E.G., UBER, LYFT)' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
@@ -11746,7 +11746,7 @@
       </c>
       <c r="F167" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE - OTHER RIDE SHARE SERVICE (LYFT, UBER, ETC.)' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE - OTHER RIDE SHARE SERVICE (LYFT, UBER, ETC.)' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
@@ -11765,7 +11765,7 @@
       </c>
       <c r="F168" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE NON-COMMERCIAL' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE NON-COMMERCIAL' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -11784,7 +11784,7 @@
       </c>
       <c r="F169" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE-COMMERCIAL' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE-COMMERCIAL' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
@@ -11803,7 +11803,7 @@
       </c>
       <c r="F170" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE-COMMERCIAL - ENTERTAINMENT/PARTY BUS' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE-COMMERCIAL - ENTERTAINMENT/PARTY BUS' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
@@ -11822,7 +11822,7 @@
       </c>
       <c r="F171" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VEHICLE-COMMERCIAL - TROLLEY BUS' ~ 'Vehicle',</v>
+        <v>(chicago_crime$location_description == 'VEHICLE-COMMERCIAL - TROLLEY BUS' ~ 'Vehicle',</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
@@ -11841,7 +11841,7 @@
       </c>
       <c r="F172" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'VESTIBULE' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'VESTIBULE' ~ 'Other',</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
@@ -11860,7 +11860,7 @@
       </c>
       <c r="F173" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'WAREHOUSE' ~ 'Business',</v>
+        <v>(chicago_crime$location_description == 'WAREHOUSE' ~ 'Business',</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -11879,7 +11879,7 @@
       </c>
       <c r="F174" t="str">
         <f t="shared" si="2"/>
-        <v>case_when(chicago_crime$location_description == 'NA' ~ 'Other',</v>
+        <v>(chicago_crime$location_description == 'NA' ~ 'Other',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>